<commit_message>
Sync up to the latest carina archetype
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/demo.xlsx
+++ b/src/test/resources/xls/demo.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10319"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D62F5460-90FE-C747-92DA-3A98E25D5425}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="18360" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GSMArena" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Execute</t>
   </si>
@@ -38,57 +39,15 @@
     <t>Samsung</t>
   </si>
   <si>
-    <t>Z2</t>
-  </si>
-  <si>
-    <t>5MP</t>
-  </si>
-  <si>
     <t>13MP</t>
   </si>
   <si>
-    <t>12MP</t>
-  </si>
-  <si>
     <t>brand</t>
   </si>
   <si>
-    <t>Galaxy S7 active</t>
-  </si>
-  <si>
-    <t>Galaxy On7 Pro</t>
-  </si>
-  <si>
     <t>model</t>
   </si>
   <si>
-    <t>4.0"</t>
-  </si>
-  <si>
-    <t>5.5"</t>
-  </si>
-  <si>
-    <t>5.1"</t>
-  </si>
-  <si>
-    <t>1GB RAM</t>
-  </si>
-  <si>
-    <t>2GB RAM</t>
-  </si>
-  <si>
-    <t>4GB RAM</t>
-  </si>
-  <si>
-    <t>1500mAh</t>
-  </si>
-  <si>
-    <t>3000mAh</t>
-  </si>
-  <si>
-    <t>4000mAh</t>
-  </si>
-  <si>
     <t>GSMA0001</t>
   </si>
   <si>
@@ -135,12 +94,48 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Galaxy S10+</t>
+  </si>
+  <si>
+    <t>16MP</t>
+  </si>
+  <si>
+    <t>3400mAh</t>
+  </si>
+  <si>
+    <t>Galaxy Fold</t>
+  </si>
+  <si>
+    <t>7.3"</t>
+  </si>
+  <si>
+    <t>12GB RAM</t>
+  </si>
+  <si>
+    <t>4380mAh</t>
+  </si>
+  <si>
+    <t>Galaxy M10</t>
+  </si>
+  <si>
+    <t>6.22"</t>
+  </si>
+  <si>
+    <t>3GB RAM</t>
+  </si>
+  <si>
+    <t>6.4"</t>
+  </si>
+  <si>
+    <t>4100mAh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,7 +187,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -208,9 +203,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -248,7 +243,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -354,7 +349,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,22 +522,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,10 +545,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -562,90 +557,90 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -656,21 +651,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,61 +673,61 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E3">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>100</v>

</xml_diff>